<commit_message>
committed ubc01 without studyfiles due to duplicates issue
</commit_message>
<xml_diff>
--- a/InputFiles/TC05_Canine_Filter_Study-UBC02.xlsx
+++ b/InputFiles/TC05_Canine_Filter_Study-UBC02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\FebBranch\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB80BCF-72F4-4653-AA77-FDBC89A0ED09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFAE18F-E6DD-4D15-A361-208A1882E8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -129,27 +129,6 @@
   coalesce(f.file_format, '') AS  Format,
   CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
   coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-WHERE s.clinical_study_designation IN ['UBC02']
-MATCH (c)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age
-RETURN  
-       coalesce(c.case_id, '') AS `Case ID`,
-       coalesce(s.clinical_study_designation, '') AS `Study Code`,
-       coalesce(s.clinical_study_type, '') AS  `Study Type`,
-       coalesce(demo.breed, '') AS Breed ,
-       coalesce(diag.disease_term, '') AS Diagnosis ,
-       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
-    coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
-       coalesce(demo.sex, '') AS Sex,
-       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
-       coalesce(diag.best_response, '') AS `Response to Treatment`,
-       coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -182,7 +161,30 @@
         coalesce(samp.sample_id, '') AS `Sample ID`,
         coalesce(c.case_id, '') AS `Case ID`,
         coalesce(demo.breed,'') AS Breed ,
-        coalesce(diag.disease_term,'') AS Diagnosis</t>
+        coalesce(diag.disease_term,'') AS Diagnosis
+order by f.file_name asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE s.clinical_study_designation IN ['UBC02']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+    coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -574,7 +576,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -608,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -642,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>

</xml_diff>